<commit_message>
funcion de lectura de archivos excel
</commit_message>
<xml_diff>
--- a/excels/customers.xlsx
+++ b/excels/customers.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Base de Datos II\streamlit\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Base de Datos II\2 Corte\excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,10 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
-  <si>
-    <t>customer_id</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>name</t>
   </si>
@@ -465,23 +462,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.7265625" customWidth="1"/>
-    <col min="2" max="2" width="17.7265625" customWidth="1"/>
-    <col min="3" max="3" width="23.08984375" customWidth="1"/>
-    <col min="4" max="4" width="26.1796875" customWidth="1"/>
-    <col min="5" max="5" width="12.36328125" customWidth="1"/>
-    <col min="7" max="7" width="24.36328125" customWidth="1"/>
+    <col min="1" max="1" width="17.7265625" customWidth="1"/>
+    <col min="2" max="2" width="23.08984375" customWidth="1"/>
+    <col min="3" max="3" width="26.1796875" customWidth="1"/>
+    <col min="4" max="4" width="12.36328125" customWidth="1"/>
+    <col min="6" max="6" width="24.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -494,132 +490,111 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3">
+        <v>123456789</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3">
-        <v>123456789</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="B3" s="3">
+        <v>987654321</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="2">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="3">
-        <v>987654321</v>
-      </c>
-      <c r="D3" s="2" t="s">
+      <c r="B4" s="3">
+        <v>111111111</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="2">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="3">
-        <v>111111111</v>
-      </c>
-      <c r="D4" s="2" t="s">
+      <c r="B5" s="3">
+        <v>222222222</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="2">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="3">
-        <v>222222222</v>
-      </c>
-      <c r="D5" s="2" t="s">
+      <c r="B6" s="3">
+        <v>333333333</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="2">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="3">
-        <v>333333333</v>
-      </c>
-      <c r="D6" s="2" t="s">
+      <c r="B7" s="3">
+        <v>444444444</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" s="2">
-        <v>6</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="3">
-        <v>444444444</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="G13" s="4"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="G14" s="5"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="G15" s="5"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="G16" s="5"/>
-    </row>
-    <row r="17" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G17" s="5"/>
-    </row>
-    <row r="18" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G18" s="5"/>
-    </row>
-    <row r="19" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G19" s="5"/>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F13" s="4"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F14" s="5"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F15" s="5"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F16" s="5"/>
+    </row>
+    <row r="17" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F17" s="5"/>
+    </row>
+    <row r="18" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F18" s="5"/>
+    </row>
+    <row r="19" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F19" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>